<commit_message>
finished my task 1.1 (without mass)
</commit_message>
<xml_diff>
--- a/data/felix/panel_properties.xlsx
+++ b/data/felix/panel_properties.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\.Uni\Project\Files\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\.Uni\Project\Git\tum-ase-project-2025\data\felix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDEA38A3-3B42-4CAC-93AF-64029878A300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{290053FF-71C3-448F-B5A5-BA002FE03F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{28511621-16EE-4FB5-BA73-910E20DD4DB3}"/>
   </bookViews>
@@ -20,48 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Element ID</t>
-  </si>
-  <si>
-    <t>Component Name</t>
   </si>
   <si>
     <t>thickness</t>
   </si>
   <si>
     <t>mass</t>
-  </si>
-  <si>
-    <t>panel1</t>
-  </si>
-  <si>
-    <t>panel2</t>
-  </si>
-  <si>
-    <t>panel3</t>
-  </si>
-  <si>
-    <t>panel4</t>
-  </si>
-  <si>
-    <t>panel5</t>
-  </si>
-  <si>
-    <t>panel6</t>
-  </si>
-  <si>
-    <t>panel7</t>
-  </si>
-  <si>
-    <t>panel8</t>
-  </si>
-  <si>
-    <t>panel9</t>
-  </si>
-  <si>
-    <t>panel10</t>
   </si>
 </sst>
 </file>
@@ -922,13 +889,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7916E014-D57F-47CB-AA34-E16614D21B29}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -938,427 +911,334 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
         <v>4</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5">
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
+      <c r="B7">
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="B8">
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
+      <c r="B9">
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
+      <c r="B10">
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
+      <c r="B11">
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
+      <c r="B12">
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
+      <c r="B13">
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>8</v>
+      <c r="B14">
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>8</v>
+      <c r="B15">
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
+      <c r="B16">
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>9</v>
+      <c r="B17">
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>9</v>
+      <c r="B18">
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>9</v>
+      <c r="B19">
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>10</v>
+      <c r="B20">
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>10</v>
+      <c r="B21">
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>10</v>
+      <c r="B22">
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>11</v>
+      <c r="B23">
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>11</v>
+      <c r="B24">
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>11</v>
+      <c r="B25">
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>12</v>
+      <c r="B26">
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>12</v>
+      <c r="B27">
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>12</v>
+      <c r="B28">
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>13</v>
+      <c r="B29">
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>13</v>
+      <c r="B30">
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>4</v>
-      </c>
-      <c r="D30">
-        <v>5.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>13</v>
+      <c r="B31">
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="D31">
         <v>5.4000000000000001E-4</v>
       </c>
     </row>

</xml_diff>